<commit_message>
Update and modernize a couple of these notebooks (e.g. replace deprecated methods)
</commit_message>
<xml_diff>
--- a/code/ch7-data-input-output/reports/TPS_report.xlsx
+++ b/code/ch7-data-input-output/reports/TPS_report.xlsx
@@ -1094,10 +1094,10 @@
     <t>price</t>
   </si>
   <si>
+    <t>sum</t>
+  </si>
+  <si>
     <t>mean</t>
-  </si>
-  <si>
-    <t>sum</t>
   </si>
   <si>
     <t>count</t>
@@ -1504,10 +1504,10 @@
         <v>359</v>
       </c>
       <c r="F2" s="1">
-        <v>510.27</v>
+        <v>510270</v>
       </c>
       <c r="G2" s="1">
-        <v>22.816</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1522,10 +1522,10 @@
         <v>360</v>
       </c>
       <c r="F3" s="1">
-        <v>510270</v>
+        <v>510.27</v>
       </c>
       <c r="G3" s="1">
-        <v>0</v>
+        <v>22.816</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -9057,10 +9057,10 @@
     <row r="1" spans="1:4">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>360</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>359</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>361</v>

</xml_diff>